<commit_message>
took my name out of the XLSX file because the script inserts the user name to the sheet every time it runs
</commit_message>
<xml_diff>
--- a/Progress_Template.xlsx
+++ b/Progress_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\git\makeprogressreport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Vacation/Sick</t>
-  </si>
-  <si>
-    <t>John Taylor</t>
   </si>
   <si>
     <t>Stimulator Development</t>
@@ -539,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -586,9 +583,7 @@
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="19"/>
       <c r="B6" s="13"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -832,9 +827,9 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>'Summary Sheet'!A6</f>
-        <v>John Taylor</v>
+        <v>0</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="9"/>
@@ -860,7 +855,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="7" t="s">
@@ -3917,9 +3912,9 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>'Summary Sheet'!A6</f>
-        <v>John Taylor</v>
+        <v>0</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="9"/>
@@ -3945,7 +3940,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="7" t="s">
@@ -7002,9 +6997,9 @@
       <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4">
         <f>'Summary Sheet'!A6</f>
-        <v>John Taylor</v>
+        <v>0</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="9"/>

</xml_diff>